<commit_message>
Completed User Story BL054 to calculate the PWV report
git-svn-id: https://sfs.atcorau.local/svn/SoftwareRepository/trunk@210 a8a9b14d-6b92-5b4b-9153-4cd90bb22c97
</commit_message>
<xml_diff>
--- a/PN022BLL/biz/Debug/BL054-AcceptanceCriteria.xlsx
+++ b/PN022BLL/biz/Debug/BL054-AcceptanceCriteria.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>PWV_09</t>
   </si>
@@ -33,9 +33,6 @@
     <t>PWV_DL1</t>
   </si>
   <si>
-    <t>SignalLength</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -51,13 +48,10 @@
     <t>CorrectedTime</t>
   </si>
   <si>
-    <t>DirectDistance</t>
-  </si>
-  <si>
-    <t>CalculatedDistance</t>
-  </si>
-  <si>
-    <t>Reworked Results</t>
+    <t>Accuracy (%)</t>
+  </si>
+  <si>
+    <t>StandardDeviation (%)</t>
   </si>
 </sst>
 </file>
@@ -73,18 +67,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,56 +383,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,28 +438,23 @@
         <v>42</v>
       </c>
       <c r="D2">
-        <v>600</v>
+        <v>9.6</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>9.6</v>
-      </c>
-      <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2" t="b">
+        <f>100*E2/D2</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="H2">
         <v>56</v>
       </c>
-      <c r="J2">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -488,264 +465,211 @@
         <v>28</v>
       </c>
       <c r="D3">
-        <v>530</v>
+        <v>11.7</v>
       </c>
       <c r="E3">
-        <v>330</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>11.7</v>
-      </c>
-      <c r="G3">
-        <v>0.9</v>
-      </c>
-      <c r="H3" t="b">
+        <f t="shared" ref="F3:F4" si="0">100*E3/D3</f>
+        <v>4.2735042735042734</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>65</v>
       </c>
-      <c r="J3">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>107.4</v>
-      </c>
-      <c r="C4" s="1">
+        <v>126</v>
+      </c>
+      <c r="C4">
         <v>87</v>
       </c>
       <c r="D4">
-        <v>740</v>
+        <v>6.3</v>
       </c>
       <c r="E4">
-        <v>540</v>
+        <v>0.7</v>
       </c>
       <c r="F4">
-        <v>6.2</v>
-      </c>
-      <c r="G4">
-        <v>3.8</v>
-      </c>
-      <c r="H4" t="b">
+        <f t="shared" si="0"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <v>58</v>
       </c>
-      <c r="J4">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>80.063903999999994</v>
+        <v>80.861557000000005</v>
       </c>
       <c r="C7">
-        <v>40.063904000000001</v>
+        <v>40.861556999999998</v>
       </c>
       <c r="D7">
-        <v>600</v>
+        <v>9.8067969999999995</v>
       </c>
       <c r="E7">
-        <v>400</v>
+        <v>0.42628961999999998</v>
       </c>
       <c r="F7">
-        <v>10.059077</v>
-      </c>
-      <c r="G7">
-        <v>0.86621720000000002</v>
-      </c>
-      <c r="H7" t="b">
+        <f t="shared" ref="F7:F9" si="1">100*E7/D7</f>
+        <v>4.3468792104088623</v>
+      </c>
+      <c r="G7" t="b">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>52.339194999999997</v>
-      </c>
-      <c r="J7">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7">
+        <v>56.263924000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>68.356949</v>
+        <v>67.484497000000005</v>
       </c>
       <c r="C8">
-        <v>28.356945</v>
+        <v>27.484497000000001</v>
       </c>
       <c r="D8">
-        <v>530</v>
+        <v>12.061915000000001</v>
       </c>
       <c r="E8">
-        <v>330</v>
+        <v>0.80147111000000004</v>
       </c>
       <c r="F8">
-        <v>12.150047000000001</v>
-      </c>
-      <c r="G8">
-        <v>2.9666603</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>63.416443000000001</v>
-      </c>
-      <c r="J8">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <f t="shared" si="1"/>
+        <v>6.6446423308405009</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>65.327667000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
-        <v>118.37050000000001</v>
+        <v>124.31859</v>
       </c>
       <c r="C9">
-        <v>78.370491000000001</v>
+        <v>84.318588000000005</v>
       </c>
       <c r="D9">
-        <v>740</v>
+        <v>6.4872775000000003</v>
       </c>
       <c r="E9">
-        <v>540</v>
+        <v>0.71557104999999999</v>
       </c>
       <c r="F9">
-        <v>8.0239171999999996</v>
-      </c>
-      <c r="G9">
-        <v>1.9985896000000001</v>
-      </c>
-      <c r="H9" t="b">
+        <f t="shared" si="1"/>
+        <v>11.030375222888182</v>
+      </c>
+      <c r="G9" t="b">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>55.749630000000003</v>
-      </c>
-      <c r="J9">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H9">
+        <v>58.082222000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>100*(B2-B7)/B2</f>
+        <v>1.3883451219512137</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:H11" si="2">100*(C2-C7)/C2</f>
+        <v>2.7105785714285768</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>-2.1541354166666657</v>
+      </c>
+      <c r="F11">
+        <f>F7-F2</f>
+        <v>0.18021254374219531</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>-0.4712928571428624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="B12">
-        <v>80.012107999999998</v>
+        <f t="shared" ref="B12:H13" si="3">100*(B3-B8)/B3</f>
+        <v>0.75809264705881674</v>
       </c>
       <c r="C12">
-        <v>40.012112000000002</v>
+        <f t="shared" si="3"/>
+        <v>1.8410821428571391</v>
       </c>
       <c r="D12">
-        <v>600</v>
-      </c>
-      <c r="E12">
-        <v>400</v>
+        <f t="shared" si="3"/>
+        <v>-3.0932905982906118</v>
       </c>
       <c r="F12">
-        <v>10.076411999999999</v>
-      </c>
-      <c r="G12">
-        <v>0.89001125000000003</v>
-      </c>
-      <c r="H12" t="b">
+        <f t="shared" ref="F12:F13" si="4">F8-F3</f>
+        <v>2.3711380573362275</v>
+      </c>
+      <c r="G12" t="b">
         <v>1</v>
       </c>
-      <c r="I12">
-        <v>52.359614999999998</v>
-      </c>
-      <c r="J12">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>-0.50410307692308498</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="B13">
-        <v>68.152832000000004</v>
+        <f t="shared" si="3"/>
+        <v>1.3344523809523807</v>
       </c>
       <c r="C13">
-        <v>28.152832</v>
+        <f t="shared" si="3"/>
+        <v>3.0820827586206834</v>
       </c>
       <c r="D13">
-        <v>530</v>
-      </c>
-      <c r="E13">
-        <v>330</v>
+        <f t="shared" si="3"/>
+        <v>-2.9726587301587371</v>
       </c>
       <c r="F13">
-        <v>12.248906</v>
-      </c>
-      <c r="G13">
-        <v>3.0059764000000002</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>63.424480000000003</v>
-      </c>
-      <c r="J13">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>106.516238</v>
-      </c>
-      <c r="C14">
-        <v>86.516227999999998</v>
-      </c>
-      <c r="D14">
-        <v>740</v>
-      </c>
-      <c r="E14">
-        <v>540</v>
-      </c>
-      <c r="F14">
-        <v>6.2774634000000002</v>
-      </c>
-      <c r="G14">
-        <v>0.4995735</v>
-      </c>
-      <c r="H14" t="b">
+        <f t="shared" si="4"/>
+        <v>-8.0735888222928764E-2</v>
+      </c>
+      <c r="G13" t="b">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>56.220908999999999</v>
-      </c>
-      <c r="J14">
-        <v>5118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="J16">
-        <v>20</v>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>-0.14176206896551996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>